<commit_message>
Update Tables, Add Average Info
</commit_message>
<xml_diff>
--- a/Boids/export_flocking.xlsx
+++ b/Boids/export_flocking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Owner\Documents\GitHub\Y3-AoAIiG-Flocking\Boids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78CFB80-9886-4937-A85B-42B14ADD81ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53018B33-CB6A-47CD-952B-F19017DB5A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Minutes Alive</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -713,7 +719,43 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.68837510936132984"/>
+                  <c:y val="0.44909444444444446"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -2352,7 +2394,43 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.67448622047244089"/>
+                  <c:y val="0.41225944444444446"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -3991,7 +4069,43 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.68236132983377074"/>
+                  <c:y val="0.36976972222222221"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -7191,14 +7305,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>3175</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>307975</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>174175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7233,8 +7347,8 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>307975</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>174175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7263,14 +7377,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>3175</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>307975</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>174175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7619,10 +7733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H201"/>
+  <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7633,7 +7747,7 @@
     <col min="7" max="8" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7659,7 +7773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7679,15 +7793,22 @@
         <v>342921</v>
       </c>
       <c r="G2">
-        <f>F2/1000</f>
+        <f t="shared" ref="G2:G33" si="0">F2/1000</f>
         <v>342.92099999999999</v>
       </c>
       <c r="H2">
-        <f>G2/60</f>
+        <f t="shared" ref="H2:H33" si="1">G2/60</f>
         <v>5.7153499999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(Table1[Seconds Alive])</f>
+        <v>217.64363790499999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -7707,15 +7828,22 @@
         <v>103627</v>
       </c>
       <c r="G3">
-        <f>F3/1000</f>
+        <f t="shared" si="0"/>
         <v>103.627</v>
       </c>
       <c r="H3">
-        <f>G3/60</f>
+        <f t="shared" si="1"/>
         <v>1.7271166666666666</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <f>STDEV(Table1[Seconds Alive])</f>
+        <v>140.68976944525295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -7735,15 +7863,15 @@
         <v>367686</v>
       </c>
       <c r="G4">
-        <f>F4/1000</f>
+        <f t="shared" si="0"/>
         <v>367.68599999999998</v>
       </c>
       <c r="H4">
-        <f>G4/60</f>
+        <f t="shared" si="1"/>
         <v>6.1280999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -7763,15 +7891,15 @@
         <v>388232</v>
       </c>
       <c r="G5">
-        <f>F5/1000</f>
+        <f t="shared" si="0"/>
         <v>388.23200000000003</v>
       </c>
       <c r="H5">
-        <f>G5/60</f>
+        <f t="shared" si="1"/>
         <v>6.4705333333333339</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7791,15 +7919,15 @@
         <v>65204</v>
       </c>
       <c r="G6">
-        <f>F6/1000</f>
+        <f t="shared" si="0"/>
         <v>65.203999999999994</v>
       </c>
       <c r="H6">
-        <f>G6/60</f>
+        <f t="shared" si="1"/>
         <v>1.0867333333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -7819,15 +7947,15 @@
         <v>334950</v>
       </c>
       <c r="G7">
-        <f>F7/1000</f>
+        <f t="shared" si="0"/>
         <v>334.95</v>
       </c>
       <c r="H7">
-        <f>G7/60</f>
+        <f t="shared" si="1"/>
         <v>5.5824999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -7847,15 +7975,15 @@
         <v>104124</v>
       </c>
       <c r="G8">
-        <f>F8/1000</f>
+        <f t="shared" si="0"/>
         <v>104.124</v>
       </c>
       <c r="H8">
-        <f>G8/60</f>
+        <f t="shared" si="1"/>
         <v>1.7353999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -7875,15 +8003,15 @@
         <v>265856</v>
       </c>
       <c r="G9">
-        <f>F9/1000</f>
+        <f t="shared" si="0"/>
         <v>265.85599999999999</v>
       </c>
       <c r="H9">
-        <f>G9/60</f>
+        <f t="shared" si="1"/>
         <v>4.4309333333333329</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -7903,15 +8031,15 @@
         <v>5124.25</v>
       </c>
       <c r="G10">
-        <f>F10/1000</f>
+        <f t="shared" si="0"/>
         <v>5.12425</v>
       </c>
       <c r="H10">
-        <f>G10/60</f>
+        <f t="shared" si="1"/>
         <v>8.540416666666667E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -7931,15 +8059,15 @@
         <v>192246</v>
       </c>
       <c r="G11">
-        <f>F11/1000</f>
+        <f t="shared" si="0"/>
         <v>192.24600000000001</v>
       </c>
       <c r="H11">
-        <f>G11/60</f>
+        <f t="shared" si="1"/>
         <v>3.2040999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -7959,15 +8087,15 @@
         <v>414213</v>
       </c>
       <c r="G12">
-        <f>F12/1000</f>
+        <f t="shared" si="0"/>
         <v>414.21300000000002</v>
       </c>
       <c r="H12">
-        <f>G12/60</f>
+        <f t="shared" si="1"/>
         <v>6.9035500000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -7987,15 +8115,15 @@
         <v>2732.42</v>
       </c>
       <c r="G13">
-        <f>F13/1000</f>
+        <f t="shared" si="0"/>
         <v>2.7324200000000003</v>
       </c>
       <c r="H13">
-        <f>G13/60</f>
+        <f t="shared" si="1"/>
         <v>4.5540333333333335E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -8015,15 +8143,15 @@
         <v>251870</v>
       </c>
       <c r="G14">
-        <f>F14/1000</f>
+        <f t="shared" si="0"/>
         <v>251.87</v>
       </c>
       <c r="H14">
-        <f>G14/60</f>
+        <f t="shared" si="1"/>
         <v>4.1978333333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -8043,15 +8171,15 @@
         <v>103855</v>
       </c>
       <c r="G15">
-        <f>F15/1000</f>
+        <f t="shared" si="0"/>
         <v>103.855</v>
       </c>
       <c r="H15">
-        <f>G15/60</f>
+        <f t="shared" si="1"/>
         <v>1.7309166666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -8071,11 +8199,11 @@
         <v>348102</v>
       </c>
       <c r="G16">
-        <f>F16/1000</f>
+        <f t="shared" si="0"/>
         <v>348.10199999999998</v>
       </c>
       <c r="H16">
-        <f>G16/60</f>
+        <f t="shared" si="1"/>
         <v>5.8016999999999994</v>
       </c>
     </row>
@@ -8099,11 +8227,11 @@
         <v>9292.9500000000007</v>
       </c>
       <c r="G17">
-        <f>F17/1000</f>
+        <f t="shared" si="0"/>
         <v>9.2929500000000012</v>
       </c>
       <c r="H17">
-        <f>G17/60</f>
+        <f t="shared" si="1"/>
         <v>0.15488250000000001</v>
       </c>
     </row>
@@ -8127,11 +8255,11 @@
         <v>461632</v>
       </c>
       <c r="G18">
-        <f>F18/1000</f>
+        <f t="shared" si="0"/>
         <v>461.63200000000001</v>
       </c>
       <c r="H18">
-        <f>G18/60</f>
+        <f t="shared" si="1"/>
         <v>7.6938666666666666</v>
       </c>
     </row>
@@ -8155,11 +8283,11 @@
         <v>176571</v>
       </c>
       <c r="G19">
-        <f>F19/1000</f>
+        <f t="shared" si="0"/>
         <v>176.571</v>
       </c>
       <c r="H19">
-        <f>G19/60</f>
+        <f t="shared" si="1"/>
         <v>2.94285</v>
       </c>
     </row>
@@ -8183,11 +8311,11 @@
         <v>312241</v>
       </c>
       <c r="G20">
-        <f>F20/1000</f>
+        <f t="shared" si="0"/>
         <v>312.24099999999999</v>
       </c>
       <c r="H20">
-        <f>G20/60</f>
+        <f t="shared" si="1"/>
         <v>5.2040166666666661</v>
       </c>
     </row>
@@ -8211,11 +8339,11 @@
         <v>374725</v>
       </c>
       <c r="G21">
-        <f>F21/1000</f>
+        <f t="shared" si="0"/>
         <v>374.72500000000002</v>
       </c>
       <c r="H21">
-        <f>G21/60</f>
+        <f t="shared" si="1"/>
         <v>6.2454166666666673</v>
       </c>
     </row>
@@ -8239,11 +8367,11 @@
         <v>8915.99</v>
       </c>
       <c r="G22">
-        <f>F22/1000</f>
+        <f t="shared" si="0"/>
         <v>8.915989999999999</v>
       </c>
       <c r="H22">
-        <f>G22/60</f>
+        <f t="shared" si="1"/>
         <v>0.14859983333333332</v>
       </c>
     </row>
@@ -8267,11 +8395,11 @@
         <v>197741</v>
       </c>
       <c r="G23">
-        <f>F23/1000</f>
+        <f t="shared" si="0"/>
         <v>197.74100000000001</v>
       </c>
       <c r="H23">
-        <f>G23/60</f>
+        <f t="shared" si="1"/>
         <v>3.2956833333333337</v>
       </c>
     </row>
@@ -8295,11 +8423,11 @@
         <v>106039</v>
       </c>
       <c r="G24">
-        <f>F24/1000</f>
+        <f t="shared" si="0"/>
         <v>106.039</v>
       </c>
       <c r="H24">
-        <f>G24/60</f>
+        <f t="shared" si="1"/>
         <v>1.7673166666666666</v>
       </c>
     </row>
@@ -8323,11 +8451,11 @@
         <v>405708</v>
       </c>
       <c r="G25">
-        <f>F25/1000</f>
+        <f t="shared" si="0"/>
         <v>405.70800000000003</v>
       </c>
       <c r="H25">
-        <f>G25/60</f>
+        <f t="shared" si="1"/>
         <v>6.7618</v>
       </c>
     </row>
@@ -8351,11 +8479,11 @@
         <v>69867.8</v>
       </c>
       <c r="G26">
-        <f>F26/1000</f>
+        <f t="shared" si="0"/>
         <v>69.867800000000003</v>
       </c>
       <c r="H26">
-        <f>G26/60</f>
+        <f t="shared" si="1"/>
         <v>1.1644633333333334</v>
       </c>
     </row>
@@ -8379,11 +8507,11 @@
         <v>357394</v>
       </c>
       <c r="G27">
-        <f>F27/1000</f>
+        <f t="shared" si="0"/>
         <v>357.39400000000001</v>
       </c>
       <c r="H27">
-        <f>G27/60</f>
+        <f t="shared" si="1"/>
         <v>5.9565666666666663</v>
       </c>
     </row>
@@ -8407,11 +8535,11 @@
         <v>379941</v>
       </c>
       <c r="G28">
-        <f>F28/1000</f>
+        <f t="shared" si="0"/>
         <v>379.94099999999997</v>
       </c>
       <c r="H28">
-        <f>G28/60</f>
+        <f t="shared" si="1"/>
         <v>6.3323499999999999</v>
       </c>
     </row>
@@ -8435,11 +8563,11 @@
         <v>254332</v>
       </c>
       <c r="G29">
-        <f>F29/1000</f>
+        <f t="shared" si="0"/>
         <v>254.33199999999999</v>
       </c>
       <c r="H29">
-        <f>G29/60</f>
+        <f t="shared" si="1"/>
         <v>4.2388666666666666</v>
       </c>
     </row>
@@ -8463,11 +8591,11 @@
         <v>189583</v>
       </c>
       <c r="G30">
-        <f>F30/1000</f>
+        <f t="shared" si="0"/>
         <v>189.583</v>
       </c>
       <c r="H30">
-        <f>G30/60</f>
+        <f t="shared" si="1"/>
         <v>3.1597166666666667</v>
       </c>
     </row>
@@ -8491,11 +8619,11 @@
         <v>320533</v>
       </c>
       <c r="G31">
-        <f>F31/1000</f>
+        <f t="shared" si="0"/>
         <v>320.53300000000002</v>
       </c>
       <c r="H31">
-        <f>G31/60</f>
+        <f t="shared" si="1"/>
         <v>5.3422166666666673</v>
       </c>
     </row>
@@ -8519,11 +8647,11 @@
         <v>276846</v>
       </c>
       <c r="G32">
-        <f>F32/1000</f>
+        <f t="shared" si="0"/>
         <v>276.846</v>
       </c>
       <c r="H32">
-        <f>G32/60</f>
+        <f t="shared" si="1"/>
         <v>4.6140999999999996</v>
       </c>
     </row>
@@ -8547,11 +8675,11 @@
         <v>333111</v>
       </c>
       <c r="G33">
-        <f>F33/1000</f>
+        <f t="shared" si="0"/>
         <v>333.11099999999999</v>
       </c>
       <c r="H33">
-        <f>G33/60</f>
+        <f t="shared" si="1"/>
         <v>5.55185</v>
       </c>
     </row>
@@ -8575,11 +8703,11 @@
         <v>277783</v>
       </c>
       <c r="G34">
-        <f>F34/1000</f>
+        <f t="shared" ref="G34:G65" si="2">F34/1000</f>
         <v>277.78300000000002</v>
       </c>
       <c r="H34">
-        <f>G34/60</f>
+        <f t="shared" ref="H34:H65" si="3">G34/60</f>
         <v>4.6297166666666669</v>
       </c>
     </row>
@@ -8603,11 +8731,11 @@
         <v>103878</v>
       </c>
       <c r="G35">
-        <f>F35/1000</f>
+        <f t="shared" si="2"/>
         <v>103.878</v>
       </c>
       <c r="H35">
-        <f>G35/60</f>
+        <f t="shared" si="3"/>
         <v>1.7313000000000001</v>
       </c>
     </row>
@@ -8631,11 +8759,11 @@
         <v>254282</v>
       </c>
       <c r="G36">
-        <f>F36/1000</f>
+        <f t="shared" si="2"/>
         <v>254.28200000000001</v>
       </c>
       <c r="H36">
-        <f>G36/60</f>
+        <f t="shared" si="3"/>
         <v>4.2380333333333331</v>
       </c>
     </row>
@@ -8659,11 +8787,11 @@
         <v>48722.7</v>
       </c>
       <c r="G37">
-        <f>F37/1000</f>
+        <f t="shared" si="2"/>
         <v>48.722699999999996</v>
       </c>
       <c r="H37">
-        <f>G37/60</f>
+        <f t="shared" si="3"/>
         <v>0.81204499999999991</v>
       </c>
     </row>
@@ -8687,11 +8815,11 @@
         <v>81002.5</v>
       </c>
       <c r="G38">
-        <f>F38/1000</f>
+        <f t="shared" si="2"/>
         <v>81.002499999999998</v>
       </c>
       <c r="H38">
-        <f>G38/60</f>
+        <f t="shared" si="3"/>
         <v>1.3500416666666666</v>
       </c>
     </row>
@@ -8715,11 +8843,11 @@
         <v>326202</v>
       </c>
       <c r="G39">
-        <f>F39/1000</f>
+        <f t="shared" si="2"/>
         <v>326.202</v>
       </c>
       <c r="H39">
-        <f>G39/60</f>
+        <f t="shared" si="3"/>
         <v>5.4367000000000001</v>
       </c>
     </row>
@@ -8743,11 +8871,11 @@
         <v>70782.7</v>
       </c>
       <c r="G40">
-        <f>F40/1000</f>
+        <f t="shared" si="2"/>
         <v>70.782699999999991</v>
       </c>
       <c r="H40">
-        <f>G40/60</f>
+        <f t="shared" si="3"/>
         <v>1.1797116666666665</v>
       </c>
     </row>
@@ -8771,11 +8899,11 @@
         <v>383279</v>
       </c>
       <c r="G41">
-        <f>F41/1000</f>
+        <f t="shared" si="2"/>
         <v>383.279</v>
       </c>
       <c r="H41">
-        <f>G41/60</f>
+        <f t="shared" si="3"/>
         <v>6.3879833333333336</v>
       </c>
     </row>
@@ -8799,11 +8927,11 @@
         <v>66235</v>
       </c>
       <c r="G42">
-        <f>F42/1000</f>
+        <f t="shared" si="2"/>
         <v>66.234999999999999</v>
       </c>
       <c r="H42">
-        <f>G42/60</f>
+        <f t="shared" si="3"/>
         <v>1.1039166666666667</v>
       </c>
     </row>
@@ -8827,11 +8955,11 @@
         <v>255935</v>
       </c>
       <c r="G43">
-        <f>F43/1000</f>
+        <f t="shared" si="2"/>
         <v>255.935</v>
       </c>
       <c r="H43">
-        <f>G43/60</f>
+        <f t="shared" si="3"/>
         <v>4.2655833333333337</v>
       </c>
     </row>
@@ -8855,11 +8983,11 @@
         <v>395699</v>
       </c>
       <c r="G44">
-        <f>F44/1000</f>
+        <f t="shared" si="2"/>
         <v>395.69900000000001</v>
       </c>
       <c r="H44">
-        <f>G44/60</f>
+        <f t="shared" si="3"/>
         <v>6.5949833333333334</v>
       </c>
     </row>
@@ -8883,11 +9011,11 @@
         <v>107170</v>
       </c>
       <c r="G45">
-        <f>F45/1000</f>
+        <f t="shared" si="2"/>
         <v>107.17</v>
       </c>
       <c r="H45">
-        <f>G45/60</f>
+        <f t="shared" si="3"/>
         <v>1.7861666666666667</v>
       </c>
     </row>
@@ -8911,11 +9039,11 @@
         <v>253809</v>
       </c>
       <c r="G46">
-        <f>F46/1000</f>
+        <f t="shared" si="2"/>
         <v>253.809</v>
       </c>
       <c r="H46">
-        <f>G46/60</f>
+        <f t="shared" si="3"/>
         <v>4.2301500000000001</v>
       </c>
     </row>
@@ -8939,11 +9067,11 @@
         <v>76404.399999999994</v>
       </c>
       <c r="G47">
-        <f>F47/1000</f>
+        <f t="shared" si="2"/>
         <v>76.404399999999995</v>
       </c>
       <c r="H47">
-        <f>G47/60</f>
+        <f t="shared" si="3"/>
         <v>1.2734066666666666</v>
       </c>
     </row>
@@ -8967,11 +9095,11 @@
         <v>338979</v>
       </c>
       <c r="G48">
-        <f>F48/1000</f>
+        <f t="shared" si="2"/>
         <v>338.97899999999998</v>
       </c>
       <c r="H48">
-        <f>G48/60</f>
+        <f t="shared" si="3"/>
         <v>5.6496499999999994</v>
       </c>
     </row>
@@ -8995,11 +9123,11 @@
         <v>63310</v>
       </c>
       <c r="G49">
-        <f>F49/1000</f>
+        <f t="shared" si="2"/>
         <v>63.31</v>
       </c>
       <c r="H49">
-        <f>G49/60</f>
+        <f t="shared" si="3"/>
         <v>1.0551666666666668</v>
       </c>
     </row>
@@ -9023,11 +9151,11 @@
         <v>135559</v>
       </c>
       <c r="G50">
-        <f>F50/1000</f>
+        <f t="shared" si="2"/>
         <v>135.559</v>
       </c>
       <c r="H50">
-        <f>G50/60</f>
+        <f t="shared" si="3"/>
         <v>2.2593166666666664</v>
       </c>
     </row>
@@ -9051,11 +9179,11 @@
         <v>331275</v>
       </c>
       <c r="G51">
-        <f>F51/1000</f>
+        <f t="shared" si="2"/>
         <v>331.27499999999998</v>
       </c>
       <c r="H51">
-        <f>G51/60</f>
+        <f t="shared" si="3"/>
         <v>5.5212499999999993</v>
       </c>
     </row>
@@ -9079,11 +9207,11 @@
         <v>289884</v>
       </c>
       <c r="G52">
-        <f>F52/1000</f>
+        <f t="shared" si="2"/>
         <v>289.88400000000001</v>
       </c>
       <c r="H52">
-        <f>G52/60</f>
+        <f t="shared" si="3"/>
         <v>4.8314000000000004</v>
       </c>
     </row>
@@ -9107,11 +9235,11 @@
         <v>306165</v>
       </c>
       <c r="G53">
-        <f>F53/1000</f>
+        <f t="shared" si="2"/>
         <v>306.16500000000002</v>
       </c>
       <c r="H53">
-        <f>G53/60</f>
+        <f t="shared" si="3"/>
         <v>5.1027500000000003</v>
       </c>
     </row>
@@ -9135,11 +9263,11 @@
         <v>102652</v>
       </c>
       <c r="G54">
-        <f>F54/1000</f>
+        <f t="shared" si="2"/>
         <v>102.652</v>
       </c>
       <c r="H54">
-        <f>G54/60</f>
+        <f t="shared" si="3"/>
         <v>1.7108666666666668</v>
       </c>
     </row>
@@ -9163,11 +9291,11 @@
         <v>32355.5</v>
       </c>
       <c r="G55">
-        <f>F55/1000</f>
+        <f t="shared" si="2"/>
         <v>32.355499999999999</v>
       </c>
       <c r="H55">
-        <f>G55/60</f>
+        <f t="shared" si="3"/>
         <v>0.53925833333333328</v>
       </c>
     </row>
@@ -9191,11 +9319,11 @@
         <v>108916</v>
       </c>
       <c r="G56">
-        <f>F56/1000</f>
+        <f t="shared" si="2"/>
         <v>108.916</v>
       </c>
       <c r="H56">
-        <f>G56/60</f>
+        <f t="shared" si="3"/>
         <v>1.8152666666666666</v>
       </c>
     </row>
@@ -9219,11 +9347,11 @@
         <v>254023</v>
       </c>
       <c r="G57">
-        <f>F57/1000</f>
+        <f t="shared" si="2"/>
         <v>254.023</v>
       </c>
       <c r="H57">
-        <f>G57/60</f>
+        <f t="shared" si="3"/>
         <v>4.233716666666667</v>
       </c>
     </row>
@@ -9247,11 +9375,11 @@
         <v>117727</v>
       </c>
       <c r="G58">
-        <f>F58/1000</f>
+        <f t="shared" si="2"/>
         <v>117.727</v>
       </c>
       <c r="H58">
-        <f>G58/60</f>
+        <f t="shared" si="3"/>
         <v>1.9621166666666667</v>
       </c>
     </row>
@@ -9275,11 +9403,11 @@
         <v>446161</v>
       </c>
       <c r="G59">
-        <f>F59/1000</f>
+        <f t="shared" si="2"/>
         <v>446.161</v>
       </c>
       <c r="H59">
-        <f>G59/60</f>
+        <f t="shared" si="3"/>
         <v>7.4360166666666663</v>
       </c>
     </row>
@@ -9303,11 +9431,11 @@
         <v>141008</v>
       </c>
       <c r="G60">
-        <f>F60/1000</f>
+        <f t="shared" si="2"/>
         <v>141.00800000000001</v>
       </c>
       <c r="H60">
-        <f>G60/60</f>
+        <f t="shared" si="3"/>
         <v>2.3501333333333334</v>
       </c>
     </row>
@@ -9331,11 +9459,11 @@
         <v>67321</v>
       </c>
       <c r="G61">
-        <f>F61/1000</f>
+        <f t="shared" si="2"/>
         <v>67.320999999999998</v>
       </c>
       <c r="H61">
-        <f>G61/60</f>
+        <f t="shared" si="3"/>
         <v>1.1220166666666667</v>
       </c>
     </row>
@@ -9359,11 +9487,11 @@
         <v>264005</v>
       </c>
       <c r="G62">
-        <f>F62/1000</f>
+        <f t="shared" si="2"/>
         <v>264.005</v>
       </c>
       <c r="H62">
-        <f>G62/60</f>
+        <f t="shared" si="3"/>
         <v>4.4000833333333329</v>
       </c>
     </row>
@@ -9387,11 +9515,11 @@
         <v>6992.08</v>
       </c>
       <c r="G63">
-        <f>F63/1000</f>
+        <f t="shared" si="2"/>
         <v>6.9920799999999996</v>
       </c>
       <c r="H63">
-        <f>G63/60</f>
+        <f t="shared" si="3"/>
         <v>0.11653466666666666</v>
       </c>
     </row>
@@ -9415,11 +9543,11 @@
         <v>92178.6</v>
       </c>
       <c r="G64">
-        <f>F64/1000</f>
+        <f t="shared" si="2"/>
         <v>92.178600000000003</v>
       </c>
       <c r="H64">
-        <f>G64/60</f>
+        <f t="shared" si="3"/>
         <v>1.5363100000000001</v>
       </c>
     </row>
@@ -9443,11 +9571,11 @@
         <v>45350.9</v>
       </c>
       <c r="G65">
-        <f>F65/1000</f>
+        <f t="shared" si="2"/>
         <v>45.350900000000003</v>
       </c>
       <c r="H65">
-        <f>G65/60</f>
+        <f t="shared" si="3"/>
         <v>0.75584833333333334</v>
       </c>
     </row>
@@ -9471,11 +9599,11 @@
         <v>289003</v>
       </c>
       <c r="G66">
-        <f>F66/1000</f>
+        <f t="shared" ref="G66:G97" si="4">F66/1000</f>
         <v>289.00299999999999</v>
       </c>
       <c r="H66">
-        <f>G66/60</f>
+        <f t="shared" ref="H66:H97" si="5">G66/60</f>
         <v>4.8167166666666663</v>
       </c>
     </row>
@@ -9499,11 +9627,11 @@
         <v>70631.199999999997</v>
       </c>
       <c r="G67">
-        <f>F67/1000</f>
+        <f t="shared" si="4"/>
         <v>70.631199999999993</v>
       </c>
       <c r="H67">
-        <f>G67/60</f>
+        <f t="shared" si="5"/>
         <v>1.1771866666666666</v>
       </c>
     </row>
@@ -9527,11 +9655,11 @@
         <v>473252</v>
       </c>
       <c r="G68">
-        <f>F68/1000</f>
+        <f t="shared" si="4"/>
         <v>473.25200000000001</v>
       </c>
       <c r="H68">
-        <f>G68/60</f>
+        <f t="shared" si="5"/>
         <v>7.8875333333333337</v>
       </c>
     </row>
@@ -9555,11 +9683,11 @@
         <v>281346</v>
       </c>
       <c r="G69">
-        <f>F69/1000</f>
+        <f t="shared" si="4"/>
         <v>281.346</v>
       </c>
       <c r="H69">
-        <f>G69/60</f>
+        <f t="shared" si="5"/>
         <v>4.6890999999999998</v>
       </c>
     </row>
@@ -9583,11 +9711,11 @@
         <v>51989.7</v>
       </c>
       <c r="G70">
-        <f>F70/1000</f>
+        <f t="shared" si="4"/>
         <v>51.989699999999999</v>
       </c>
       <c r="H70">
-        <f>G70/60</f>
+        <f t="shared" si="5"/>
         <v>0.86649500000000002</v>
       </c>
     </row>
@@ -9611,11 +9739,11 @@
         <v>351157</v>
       </c>
       <c r="G71">
-        <f>F71/1000</f>
+        <f t="shared" si="4"/>
         <v>351.15699999999998</v>
       </c>
       <c r="H71">
-        <f>G71/60</f>
+        <f t="shared" si="5"/>
         <v>5.8526166666666661</v>
       </c>
     </row>
@@ -9639,11 +9767,11 @@
         <v>103160</v>
       </c>
       <c r="G72">
-        <f>F72/1000</f>
+        <f t="shared" si="4"/>
         <v>103.16</v>
       </c>
       <c r="H72">
-        <f>G72/60</f>
+        <f t="shared" si="5"/>
         <v>1.7193333333333334</v>
       </c>
     </row>
@@ -9667,11 +9795,11 @@
         <v>315048</v>
       </c>
       <c r="G73">
-        <f>F73/1000</f>
+        <f t="shared" si="4"/>
         <v>315.048</v>
       </c>
       <c r="H73">
-        <f>G73/60</f>
+        <f t="shared" si="5"/>
         <v>5.2507999999999999</v>
       </c>
     </row>
@@ -9695,11 +9823,11 @@
         <v>240111</v>
       </c>
       <c r="G74">
-        <f>F74/1000</f>
+        <f t="shared" si="4"/>
         <v>240.11099999999999</v>
       </c>
       <c r="H74">
-        <f>G74/60</f>
+        <f t="shared" si="5"/>
         <v>4.0018500000000001</v>
       </c>
     </row>
@@ -9723,11 +9851,11 @@
         <v>341188</v>
       </c>
       <c r="G75">
-        <f>F75/1000</f>
+        <f t="shared" si="4"/>
         <v>341.18799999999999</v>
       </c>
       <c r="H75">
-        <f>G75/60</f>
+        <f t="shared" si="5"/>
         <v>5.6864666666666661</v>
       </c>
     </row>
@@ -9751,11 +9879,11 @@
         <v>398141</v>
       </c>
       <c r="G76">
-        <f>F76/1000</f>
+        <f t="shared" si="4"/>
         <v>398.14100000000002</v>
       </c>
       <c r="H76">
-        <f>G76/60</f>
+        <f t="shared" si="5"/>
         <v>6.6356833333333336</v>
       </c>
     </row>
@@ -9779,11 +9907,11 @@
         <v>29441.4</v>
       </c>
       <c r="G77">
-        <f>F77/1000</f>
+        <f t="shared" si="4"/>
         <v>29.441400000000002</v>
       </c>
       <c r="H77">
-        <f>G77/60</f>
+        <f t="shared" si="5"/>
         <v>0.49069000000000002</v>
       </c>
     </row>
@@ -9807,11 +9935,11 @@
         <v>84924.7</v>
       </c>
       <c r="G78">
-        <f>F78/1000</f>
+        <f t="shared" si="4"/>
         <v>84.924700000000001</v>
       </c>
       <c r="H78">
-        <f>G78/60</f>
+        <f t="shared" si="5"/>
         <v>1.4154116666666667</v>
       </c>
     </row>
@@ -9835,11 +9963,11 @@
         <v>226125</v>
       </c>
       <c r="G79">
-        <f>F79/1000</f>
+        <f t="shared" si="4"/>
         <v>226.125</v>
       </c>
       <c r="H79">
-        <f>G79/60</f>
+        <f t="shared" si="5"/>
         <v>3.7687499999999998</v>
       </c>
     </row>
@@ -9863,11 +9991,11 @@
         <v>407076</v>
       </c>
       <c r="G80">
-        <f>F80/1000</f>
+        <f t="shared" si="4"/>
         <v>407.07600000000002</v>
       </c>
       <c r="H80">
-        <f>G80/60</f>
+        <f t="shared" si="5"/>
         <v>6.7846000000000002</v>
       </c>
     </row>
@@ -9891,11 +10019,11 @@
         <v>311218</v>
       </c>
       <c r="G81">
-        <f>F81/1000</f>
+        <f t="shared" si="4"/>
         <v>311.21800000000002</v>
       </c>
       <c r="H81">
-        <f>G81/60</f>
+        <f t="shared" si="5"/>
         <v>5.1869666666666667</v>
       </c>
     </row>
@@ -9919,11 +10047,11 @@
         <v>411201</v>
       </c>
       <c r="G82">
-        <f>F82/1000</f>
+        <f t="shared" si="4"/>
         <v>411.20100000000002</v>
       </c>
       <c r="H82">
-        <f>G82/60</f>
+        <f t="shared" si="5"/>
         <v>6.8533500000000007</v>
       </c>
     </row>
@@ -9947,11 +10075,11 @@
         <v>236343</v>
       </c>
       <c r="G83">
-        <f>F83/1000</f>
+        <f t="shared" si="4"/>
         <v>236.34299999999999</v>
       </c>
       <c r="H83">
-        <f>G83/60</f>
+        <f t="shared" si="5"/>
         <v>3.9390499999999999</v>
       </c>
     </row>
@@ -9975,11 +10103,11 @@
         <v>268514</v>
       </c>
       <c r="G84">
-        <f>F84/1000</f>
+        <f t="shared" si="4"/>
         <v>268.51400000000001</v>
       </c>
       <c r="H84">
-        <f>G84/60</f>
+        <f t="shared" si="5"/>
         <v>4.4752333333333336</v>
       </c>
     </row>
@@ -10003,11 +10131,11 @@
         <v>167936</v>
       </c>
       <c r="G85">
-        <f>F85/1000</f>
+        <f t="shared" si="4"/>
         <v>167.93600000000001</v>
       </c>
       <c r="H85">
-        <f>G85/60</f>
+        <f t="shared" si="5"/>
         <v>2.7989333333333333</v>
       </c>
     </row>
@@ -10031,11 +10159,11 @@
         <v>106406</v>
       </c>
       <c r="G86">
-        <f>F86/1000</f>
+        <f t="shared" si="4"/>
         <v>106.40600000000001</v>
       </c>
       <c r="H86">
-        <f>G86/60</f>
+        <f t="shared" si="5"/>
         <v>1.7734333333333334</v>
       </c>
     </row>
@@ -10059,11 +10187,11 @@
         <v>209733</v>
       </c>
       <c r="G87">
-        <f>F87/1000</f>
+        <f t="shared" si="4"/>
         <v>209.733</v>
       </c>
       <c r="H87">
-        <f>G87/60</f>
+        <f t="shared" si="5"/>
         <v>3.4955500000000002</v>
       </c>
     </row>
@@ -10087,11 +10215,11 @@
         <v>58046.6</v>
       </c>
       <c r="G88">
-        <f>F88/1000</f>
+        <f t="shared" si="4"/>
         <v>58.046599999999998</v>
       </c>
       <c r="H88">
-        <f>G88/60</f>
+        <f t="shared" si="5"/>
         <v>0.96744333333333332</v>
       </c>
     </row>
@@ -10115,11 +10243,11 @@
         <v>349481</v>
       </c>
       <c r="G89">
-        <f>F89/1000</f>
+        <f t="shared" si="4"/>
         <v>349.48099999999999</v>
       </c>
       <c r="H89">
-        <f>G89/60</f>
+        <f t="shared" si="5"/>
         <v>5.8246833333333337</v>
       </c>
     </row>
@@ -10143,11 +10271,11 @@
         <v>57436.9</v>
       </c>
       <c r="G90">
-        <f>F90/1000</f>
+        <f t="shared" si="4"/>
         <v>57.436900000000001</v>
       </c>
       <c r="H90">
-        <f>G90/60</f>
+        <f t="shared" si="5"/>
         <v>0.9572816666666667</v>
       </c>
     </row>
@@ -10171,11 +10299,11 @@
         <v>279262</v>
       </c>
       <c r="G91">
-        <f>F91/1000</f>
+        <f t="shared" si="4"/>
         <v>279.262</v>
       </c>
       <c r="H91">
-        <f>G91/60</f>
+        <f t="shared" si="5"/>
         <v>4.6543666666666663</v>
       </c>
     </row>
@@ -10199,11 +10327,11 @@
         <v>146810</v>
       </c>
       <c r="G92">
-        <f>F92/1000</f>
+        <f t="shared" si="4"/>
         <v>146.81</v>
       </c>
       <c r="H92">
-        <f>G92/60</f>
+        <f t="shared" si="5"/>
         <v>2.4468333333333332</v>
       </c>
     </row>
@@ -10227,11 +10355,11 @@
         <v>350261</v>
       </c>
       <c r="G93">
-        <f>F93/1000</f>
+        <f t="shared" si="4"/>
         <v>350.26100000000002</v>
       </c>
       <c r="H93">
-        <f>G93/60</f>
+        <f t="shared" si="5"/>
         <v>5.8376833333333336</v>
       </c>
     </row>
@@ -10255,11 +10383,11 @@
         <v>216902</v>
       </c>
       <c r="G94">
-        <f>F94/1000</f>
+        <f t="shared" si="4"/>
         <v>216.90199999999999</v>
       </c>
       <c r="H94">
-        <f>G94/60</f>
+        <f t="shared" si="5"/>
         <v>3.6150333333333333</v>
       </c>
     </row>
@@ -10283,11 +10411,11 @@
         <v>254448</v>
       </c>
       <c r="G95">
-        <f>F95/1000</f>
+        <f t="shared" si="4"/>
         <v>254.44800000000001</v>
       </c>
       <c r="H95">
-        <f>G95/60</f>
+        <f t="shared" si="5"/>
         <v>4.2408000000000001</v>
       </c>
     </row>
@@ -10311,11 +10439,11 @@
         <v>325963</v>
       </c>
       <c r="G96">
-        <f>F96/1000</f>
+        <f t="shared" si="4"/>
         <v>325.96300000000002</v>
       </c>
       <c r="H96">
-        <f>G96/60</f>
+        <f t="shared" si="5"/>
         <v>5.4327166666666669</v>
       </c>
     </row>
@@ -10339,11 +10467,11 @@
         <v>304947</v>
       </c>
       <c r="G97">
-        <f>F97/1000</f>
+        <f t="shared" si="4"/>
         <v>304.947</v>
       </c>
       <c r="H97">
-        <f>G97/60</f>
+        <f t="shared" si="5"/>
         <v>5.0824499999999997</v>
       </c>
     </row>
@@ -10367,11 +10495,11 @@
         <v>409290</v>
       </c>
       <c r="G98">
-        <f>F98/1000</f>
+        <f t="shared" ref="G98:G129" si="6">F98/1000</f>
         <v>409.29</v>
       </c>
       <c r="H98">
-        <f>G98/60</f>
+        <f t="shared" ref="H98:H129" si="7">G98/60</f>
         <v>6.8215000000000003</v>
       </c>
     </row>
@@ -10395,11 +10523,11 @@
         <v>129620</v>
       </c>
       <c r="G99">
-        <f>F99/1000</f>
+        <f t="shared" si="6"/>
         <v>129.62</v>
       </c>
       <c r="H99">
-        <f>G99/60</f>
+        <f t="shared" si="7"/>
         <v>2.1603333333333334</v>
       </c>
     </row>
@@ -10423,11 +10551,11 @@
         <v>412102</v>
       </c>
       <c r="G100">
-        <f>F100/1000</f>
+        <f t="shared" si="6"/>
         <v>412.10199999999998</v>
       </c>
       <c r="H100">
-        <f>G100/60</f>
+        <f t="shared" si="7"/>
         <v>6.8683666666666658</v>
       </c>
     </row>
@@ -10451,11 +10579,11 @@
         <v>114870</v>
       </c>
       <c r="G101">
-        <f>F101/1000</f>
+        <f t="shared" si="6"/>
         <v>114.87</v>
       </c>
       <c r="H101">
-        <f>G101/60</f>
+        <f t="shared" si="7"/>
         <v>1.9145000000000001</v>
       </c>
     </row>
@@ -10479,11 +10607,11 @@
         <v>357305</v>
       </c>
       <c r="G102">
-        <f>F102/1000</f>
+        <f t="shared" si="6"/>
         <v>357.30500000000001</v>
       </c>
       <c r="H102">
-        <f>G102/60</f>
+        <f t="shared" si="7"/>
         <v>5.9550833333333335</v>
       </c>
     </row>
@@ -10507,11 +10635,11 @@
         <v>159978</v>
       </c>
       <c r="G103">
-        <f>F103/1000</f>
+        <f t="shared" si="6"/>
         <v>159.97800000000001</v>
       </c>
       <c r="H103">
-        <f>G103/60</f>
+        <f t="shared" si="7"/>
         <v>2.6663000000000001</v>
       </c>
     </row>
@@ -10535,11 +10663,11 @@
         <v>113572</v>
       </c>
       <c r="G104">
-        <f>F104/1000</f>
+        <f t="shared" si="6"/>
         <v>113.572</v>
       </c>
       <c r="H104">
-        <f>G104/60</f>
+        <f t="shared" si="7"/>
         <v>1.8928666666666667</v>
       </c>
     </row>
@@ -10563,11 +10691,11 @@
         <v>291413</v>
       </c>
       <c r="G105">
-        <f>F105/1000</f>
+        <f t="shared" si="6"/>
         <v>291.41300000000001</v>
       </c>
       <c r="H105">
-        <f>G105/60</f>
+        <f t="shared" si="7"/>
         <v>4.8568833333333332</v>
       </c>
     </row>
@@ -10591,11 +10719,11 @@
         <v>355960</v>
       </c>
       <c r="G106">
-        <f>F106/1000</f>
+        <f t="shared" si="6"/>
         <v>355.96</v>
       </c>
       <c r="H106">
-        <f>G106/60</f>
+        <f t="shared" si="7"/>
         <v>5.9326666666666661</v>
       </c>
     </row>
@@ -10619,11 +10747,11 @@
         <v>159618</v>
       </c>
       <c r="G107">
-        <f>F107/1000</f>
+        <f t="shared" si="6"/>
         <v>159.61799999999999</v>
       </c>
       <c r="H107">
-        <f>G107/60</f>
+        <f t="shared" si="7"/>
         <v>2.6602999999999999</v>
       </c>
     </row>
@@ -10647,11 +10775,11 @@
         <v>199304</v>
       </c>
       <c r="G108">
-        <f>F108/1000</f>
+        <f t="shared" si="6"/>
         <v>199.304</v>
       </c>
       <c r="H108">
-        <f>G108/60</f>
+        <f t="shared" si="7"/>
         <v>3.3217333333333334</v>
       </c>
     </row>
@@ -10675,11 +10803,11 @@
         <v>119649</v>
       </c>
       <c r="G109">
-        <f>F109/1000</f>
+        <f t="shared" si="6"/>
         <v>119.649</v>
       </c>
       <c r="H109">
-        <f>G109/60</f>
+        <f t="shared" si="7"/>
         <v>1.9941500000000001</v>
       </c>
     </row>
@@ -10703,11 +10831,11 @@
         <v>101853</v>
       </c>
       <c r="G110">
-        <f>F110/1000</f>
+        <f t="shared" si="6"/>
         <v>101.85299999999999</v>
       </c>
       <c r="H110">
-        <f>G110/60</f>
+        <f t="shared" si="7"/>
         <v>1.6975499999999999</v>
       </c>
     </row>
@@ -10731,11 +10859,11 @@
         <v>372380</v>
       </c>
       <c r="G111">
-        <f>F111/1000</f>
+        <f t="shared" si="6"/>
         <v>372.38</v>
       </c>
       <c r="H111">
-        <f>G111/60</f>
+        <f t="shared" si="7"/>
         <v>6.2063333333333333</v>
       </c>
     </row>
@@ -10759,11 +10887,11 @@
         <v>71164.100000000006</v>
       </c>
       <c r="G112">
-        <f>F112/1000</f>
+        <f t="shared" si="6"/>
         <v>71.164100000000005</v>
       </c>
       <c r="H112">
-        <f>G112/60</f>
+        <f t="shared" si="7"/>
         <v>1.1860683333333335</v>
       </c>
     </row>
@@ -10787,11 +10915,11 @@
         <v>95226.8</v>
       </c>
       <c r="G113">
-        <f>F113/1000</f>
+        <f t="shared" si="6"/>
         <v>95.226799999999997</v>
       </c>
       <c r="H113">
-        <f>G113/60</f>
+        <f t="shared" si="7"/>
         <v>1.5871133333333334</v>
       </c>
     </row>
@@ -10815,11 +10943,11 @@
         <v>161912</v>
       </c>
       <c r="G114">
-        <f>F114/1000</f>
+        <f t="shared" si="6"/>
         <v>161.91200000000001</v>
       </c>
       <c r="H114">
-        <f>G114/60</f>
+        <f t="shared" si="7"/>
         <v>2.6985333333333332</v>
       </c>
     </row>
@@ -10843,11 +10971,11 @@
         <v>114162</v>
       </c>
       <c r="G115">
-        <f>F115/1000</f>
+        <f t="shared" si="6"/>
         <v>114.16200000000001</v>
       </c>
       <c r="H115">
-        <f>G115/60</f>
+        <f t="shared" si="7"/>
         <v>1.9027000000000001</v>
       </c>
     </row>
@@ -10871,11 +10999,11 @@
         <v>13648.7</v>
       </c>
       <c r="G116">
-        <f>F116/1000</f>
+        <f t="shared" si="6"/>
         <v>13.648700000000002</v>
       </c>
       <c r="H116">
-        <f>G116/60</f>
+        <f t="shared" si="7"/>
         <v>0.22747833333333337</v>
       </c>
     </row>
@@ -10899,11 +11027,11 @@
         <v>412629</v>
       </c>
       <c r="G117">
-        <f>F117/1000</f>
+        <f t="shared" si="6"/>
         <v>412.62900000000002</v>
       </c>
       <c r="H117">
-        <f>G117/60</f>
+        <f t="shared" si="7"/>
         <v>6.8771500000000003</v>
       </c>
     </row>
@@ -10927,11 +11055,11 @@
         <v>235176</v>
       </c>
       <c r="G118">
-        <f>F118/1000</f>
+        <f t="shared" si="6"/>
         <v>235.17599999999999</v>
       </c>
       <c r="H118">
-        <f>G118/60</f>
+        <f t="shared" si="7"/>
         <v>3.9196</v>
       </c>
     </row>
@@ -10955,11 +11083,11 @@
         <v>178426</v>
       </c>
       <c r="G119">
-        <f>F119/1000</f>
+        <f t="shared" si="6"/>
         <v>178.42599999999999</v>
       </c>
       <c r="H119">
-        <f>G119/60</f>
+        <f t="shared" si="7"/>
         <v>2.9737666666666667</v>
       </c>
     </row>
@@ -10983,11 +11111,11 @@
         <v>158286</v>
       </c>
       <c r="G120">
-        <f>F120/1000</f>
+        <f t="shared" si="6"/>
         <v>158.286</v>
       </c>
       <c r="H120">
-        <f>G120/60</f>
+        <f t="shared" si="7"/>
         <v>2.6381000000000001</v>
       </c>
     </row>
@@ -11011,11 +11139,11 @@
         <v>170332</v>
       </c>
       <c r="G121">
-        <f>F121/1000</f>
+        <f t="shared" si="6"/>
         <v>170.33199999999999</v>
       </c>
       <c r="H121">
-        <f>G121/60</f>
+        <f t="shared" si="7"/>
         <v>2.8388666666666666</v>
       </c>
     </row>
@@ -11039,11 +11167,11 @@
         <v>101.459</v>
       </c>
       <c r="G122">
-        <f>F122/1000</f>
+        <f t="shared" si="6"/>
         <v>0.10145900000000001</v>
       </c>
       <c r="H122">
-        <f>G122/60</f>
+        <f t="shared" si="7"/>
         <v>1.6909833333333334E-3</v>
       </c>
     </row>
@@ -11067,11 +11195,11 @@
         <v>928.56899999999996</v>
       </c>
       <c r="G123">
-        <f>F123/1000</f>
+        <f t="shared" si="6"/>
         <v>0.92856899999999998</v>
       </c>
       <c r="H123">
-        <f>G123/60</f>
+        <f t="shared" si="7"/>
         <v>1.5476149999999999E-2</v>
       </c>
     </row>
@@ -11095,11 +11223,11 @@
         <v>521423</v>
       </c>
       <c r="G124">
-        <f>F124/1000</f>
+        <f t="shared" si="6"/>
         <v>521.423</v>
       </c>
       <c r="H124">
-        <f>G124/60</f>
+        <f t="shared" si="7"/>
         <v>8.6903833333333331</v>
       </c>
     </row>
@@ -11123,11 +11251,11 @@
         <v>441001</v>
       </c>
       <c r="G125">
-        <f>F125/1000</f>
+        <f t="shared" si="6"/>
         <v>441.00099999999998</v>
       </c>
       <c r="H125">
-        <f>G125/60</f>
+        <f t="shared" si="7"/>
         <v>7.350016666666666</v>
       </c>
     </row>
@@ -11151,11 +11279,11 @@
         <v>337080</v>
       </c>
       <c r="G126">
-        <f>F126/1000</f>
+        <f t="shared" si="6"/>
         <v>337.08</v>
       </c>
       <c r="H126">
-        <f>G126/60</f>
+        <f t="shared" si="7"/>
         <v>5.6179999999999994</v>
       </c>
     </row>
@@ -11179,11 +11307,11 @@
         <v>11723.5</v>
       </c>
       <c r="G127">
-        <f>F127/1000</f>
+        <f t="shared" si="6"/>
         <v>11.7235</v>
       </c>
       <c r="H127">
-        <f>G127/60</f>
+        <f t="shared" si="7"/>
         <v>0.19539166666666666</v>
       </c>
     </row>
@@ -11207,11 +11335,11 @@
         <v>275892</v>
       </c>
       <c r="G128">
-        <f>F128/1000</f>
+        <f t="shared" si="6"/>
         <v>275.892</v>
       </c>
       <c r="H128">
-        <f>G128/60</f>
+        <f t="shared" si="7"/>
         <v>4.5982000000000003</v>
       </c>
     </row>
@@ -11235,11 +11363,11 @@
         <v>272657</v>
       </c>
       <c r="G129">
-        <f>F129/1000</f>
+        <f t="shared" si="6"/>
         <v>272.65699999999998</v>
       </c>
       <c r="H129">
-        <f>G129/60</f>
+        <f t="shared" si="7"/>
         <v>4.5442833333333335</v>
       </c>
     </row>
@@ -11263,11 +11391,11 @@
         <v>205751</v>
       </c>
       <c r="G130">
-        <f>F130/1000</f>
+        <f t="shared" ref="G130:G161" si="8">F130/1000</f>
         <v>205.751</v>
       </c>
       <c r="H130">
-        <f>G130/60</f>
+        <f t="shared" ref="H130:H161" si="9">G130/60</f>
         <v>3.4291833333333335</v>
       </c>
     </row>
@@ -11291,11 +11419,11 @@
         <v>112470</v>
       </c>
       <c r="G131">
-        <f>F131/1000</f>
+        <f t="shared" si="8"/>
         <v>112.47</v>
       </c>
       <c r="H131">
-        <f>G131/60</f>
+        <f t="shared" si="9"/>
         <v>1.8745000000000001</v>
       </c>
     </row>
@@ -11319,11 +11447,11 @@
         <v>235906</v>
       </c>
       <c r="G132">
-        <f>F132/1000</f>
+        <f t="shared" si="8"/>
         <v>235.90600000000001</v>
       </c>
       <c r="H132">
-        <f>G132/60</f>
+        <f t="shared" si="9"/>
         <v>3.9317666666666669</v>
       </c>
     </row>
@@ -11347,11 +11475,11 @@
         <v>122221</v>
       </c>
       <c r="G133">
-        <f>F133/1000</f>
+        <f t="shared" si="8"/>
         <v>122.221</v>
       </c>
       <c r="H133">
-        <f>G133/60</f>
+        <f t="shared" si="9"/>
         <v>2.0370166666666667</v>
       </c>
     </row>
@@ -11375,11 +11503,11 @@
         <v>11923.9</v>
       </c>
       <c r="G134">
-        <f>F134/1000</f>
+        <f t="shared" si="8"/>
         <v>11.9239</v>
       </c>
       <c r="H134">
-        <f>G134/60</f>
+        <f t="shared" si="9"/>
         <v>0.19873166666666667</v>
       </c>
     </row>
@@ -11403,11 +11531,11 @@
         <v>103033</v>
       </c>
       <c r="G135">
-        <f>F135/1000</f>
+        <f t="shared" si="8"/>
         <v>103.033</v>
       </c>
       <c r="H135">
-        <f>G135/60</f>
+        <f t="shared" si="9"/>
         <v>1.7172166666666666</v>
       </c>
     </row>
@@ -11431,11 +11559,11 @@
         <v>539185</v>
       </c>
       <c r="G136">
-        <f>F136/1000</f>
+        <f t="shared" si="8"/>
         <v>539.18499999999995</v>
       </c>
       <c r="H136">
-        <f>G136/60</f>
+        <f t="shared" si="9"/>
         <v>8.9864166666666652</v>
       </c>
     </row>
@@ -11459,11 +11587,11 @@
         <v>322732</v>
       </c>
       <c r="G137">
-        <f>F137/1000</f>
+        <f t="shared" si="8"/>
         <v>322.73200000000003</v>
       </c>
       <c r="H137">
-        <f>G137/60</f>
+        <f t="shared" si="9"/>
         <v>5.3788666666666671</v>
       </c>
     </row>
@@ -11487,11 +11615,11 @@
         <v>11485.7</v>
       </c>
       <c r="G138">
-        <f>F138/1000</f>
+        <f t="shared" si="8"/>
         <v>11.485700000000001</v>
       </c>
       <c r="H138">
-        <f>G138/60</f>
+        <f t="shared" si="9"/>
         <v>0.19142833333333337</v>
       </c>
     </row>
@@ -11515,11 +11643,11 @@
         <v>102923</v>
       </c>
       <c r="G139">
-        <f>F139/1000</f>
+        <f t="shared" si="8"/>
         <v>102.923</v>
       </c>
       <c r="H139">
-        <f>G139/60</f>
+        <f t="shared" si="9"/>
         <v>1.7153833333333333</v>
       </c>
     </row>
@@ -11543,11 +11671,11 @@
         <v>328684</v>
       </c>
       <c r="G140">
-        <f>F140/1000</f>
+        <f t="shared" si="8"/>
         <v>328.68400000000003</v>
       </c>
       <c r="H140">
-        <f>G140/60</f>
+        <f t="shared" si="9"/>
         <v>5.4780666666666669</v>
       </c>
     </row>
@@ -11571,11 +11699,11 @@
         <v>35110.199999999997</v>
       </c>
       <c r="G141">
-        <f>F141/1000</f>
+        <f t="shared" si="8"/>
         <v>35.110199999999999</v>
       </c>
       <c r="H141">
-        <f>G141/60</f>
+        <f t="shared" si="9"/>
         <v>0.58516999999999997</v>
       </c>
     </row>
@@ -11599,11 +11727,11 @@
         <v>325871</v>
       </c>
       <c r="G142">
-        <f>F142/1000</f>
+        <f t="shared" si="8"/>
         <v>325.87099999999998</v>
       </c>
       <c r="H142">
-        <f>G142/60</f>
+        <f t="shared" si="9"/>
         <v>5.4311833333333333</v>
       </c>
     </row>
@@ -11627,11 +11755,11 @@
         <v>116951</v>
       </c>
       <c r="G143">
-        <f>F143/1000</f>
+        <f t="shared" si="8"/>
         <v>116.95099999999999</v>
       </c>
       <c r="H143">
-        <f>G143/60</f>
+        <f t="shared" si="9"/>
         <v>1.9491833333333333</v>
       </c>
     </row>
@@ -11655,11 +11783,11 @@
         <v>30937.8</v>
       </c>
       <c r="G144">
-        <f>F144/1000</f>
+        <f t="shared" si="8"/>
         <v>30.937799999999999</v>
       </c>
       <c r="H144">
-        <f>G144/60</f>
+        <f t="shared" si="9"/>
         <v>0.51563000000000003</v>
       </c>
     </row>
@@ -11683,11 +11811,11 @@
         <v>57890</v>
       </c>
       <c r="G145">
-        <f>F145/1000</f>
+        <f t="shared" si="8"/>
         <v>57.89</v>
       </c>
       <c r="H145">
-        <f>G145/60</f>
+        <f t="shared" si="9"/>
         <v>0.96483333333333332</v>
       </c>
     </row>
@@ -11711,11 +11839,11 @@
         <v>78842.899999999994</v>
       </c>
       <c r="G146">
-        <f>F146/1000</f>
+        <f t="shared" si="8"/>
         <v>78.8429</v>
       </c>
       <c r="H146">
-        <f>G146/60</f>
+        <f t="shared" si="9"/>
         <v>1.3140483333333333</v>
       </c>
     </row>
@@ -11739,11 +11867,11 @@
         <v>254683</v>
       </c>
       <c r="G147">
-        <f>F147/1000</f>
+        <f t="shared" si="8"/>
         <v>254.68299999999999</v>
       </c>
       <c r="H147">
-        <f>G147/60</f>
+        <f t="shared" si="9"/>
         <v>4.2447166666666662</v>
       </c>
     </row>
@@ -11767,11 +11895,11 @@
         <v>214871</v>
       </c>
       <c r="G148">
-        <f>F148/1000</f>
+        <f t="shared" si="8"/>
         <v>214.87100000000001</v>
       </c>
       <c r="H148">
-        <f>G148/60</f>
+        <f t="shared" si="9"/>
         <v>3.5811833333333336</v>
       </c>
     </row>
@@ -11795,11 +11923,11 @@
         <v>425541</v>
       </c>
       <c r="G149">
-        <f>F149/1000</f>
+        <f t="shared" si="8"/>
         <v>425.541</v>
       </c>
       <c r="H149">
-        <f>G149/60</f>
+        <f t="shared" si="9"/>
         <v>7.0923499999999997</v>
       </c>
     </row>
@@ -11823,11 +11951,11 @@
         <v>44358.1</v>
       </c>
       <c r="G150">
-        <f>F150/1000</f>
+        <f t="shared" si="8"/>
         <v>44.3581</v>
       </c>
       <c r="H150">
-        <f>G150/60</f>
+        <f t="shared" si="9"/>
         <v>0.73930166666666663</v>
       </c>
     </row>
@@ -11851,11 +11979,11 @@
         <v>566728</v>
       </c>
       <c r="G151">
-        <f>F151/1000</f>
+        <f t="shared" si="8"/>
         <v>566.72799999999995</v>
       </c>
       <c r="H151">
-        <f>G151/60</f>
+        <f t="shared" si="9"/>
         <v>9.4454666666666665</v>
       </c>
     </row>
@@ -11879,11 +12007,11 @@
         <v>313228</v>
       </c>
       <c r="G152">
-        <f>F152/1000</f>
+        <f t="shared" si="8"/>
         <v>313.22800000000001</v>
       </c>
       <c r="H152">
-        <f>G152/60</f>
+        <f t="shared" si="9"/>
         <v>5.2204666666666668</v>
       </c>
     </row>
@@ -11907,11 +12035,11 @@
         <v>312275</v>
       </c>
       <c r="G153">
-        <f>F153/1000</f>
+        <f t="shared" si="8"/>
         <v>312.27499999999998</v>
       </c>
       <c r="H153">
-        <f>G153/60</f>
+        <f t="shared" si="9"/>
         <v>5.2045833333333329</v>
       </c>
     </row>
@@ -11935,11 +12063,11 @@
         <v>61060.6</v>
       </c>
       <c r="G154">
-        <f>F154/1000</f>
+        <f t="shared" si="8"/>
         <v>61.060600000000001</v>
       </c>
       <c r="H154">
-        <f>G154/60</f>
+        <f t="shared" si="9"/>
         <v>1.0176766666666668</v>
       </c>
     </row>
@@ -11963,11 +12091,11 @@
         <v>254103</v>
       </c>
       <c r="G155">
-        <f>F155/1000</f>
+        <f t="shared" si="8"/>
         <v>254.10300000000001</v>
       </c>
       <c r="H155">
-        <f>G155/60</f>
+        <f t="shared" si="9"/>
         <v>4.2350500000000002</v>
       </c>
     </row>
@@ -11991,11 +12119,11 @@
         <v>96026.7</v>
       </c>
       <c r="G156">
-        <f>F156/1000</f>
+        <f t="shared" si="8"/>
         <v>96.026699999999991</v>
       </c>
       <c r="H156">
-        <f>G156/60</f>
+        <f t="shared" si="9"/>
         <v>1.6004449999999999</v>
       </c>
     </row>
@@ -12019,11 +12147,11 @@
         <v>481789</v>
       </c>
       <c r="G157">
-        <f>F157/1000</f>
+        <f t="shared" si="8"/>
         <v>481.78899999999999</v>
       </c>
       <c r="H157">
-        <f>G157/60</f>
+        <f t="shared" si="9"/>
         <v>8.029816666666667</v>
       </c>
     </row>
@@ -12047,11 +12175,11 @@
         <v>305273</v>
       </c>
       <c r="G158">
-        <f>F158/1000</f>
+        <f t="shared" si="8"/>
         <v>305.27300000000002</v>
       </c>
       <c r="H158">
-        <f>G158/60</f>
+        <f t="shared" si="9"/>
         <v>5.087883333333334</v>
       </c>
     </row>
@@ -12075,11 +12203,11 @@
         <v>9808.57</v>
       </c>
       <c r="G159">
-        <f>F159/1000</f>
+        <f t="shared" si="8"/>
         <v>9.8085699999999996</v>
       </c>
       <c r="H159">
-        <f>G159/60</f>
+        <f t="shared" si="9"/>
         <v>0.16347616666666667</v>
       </c>
     </row>
@@ -12103,11 +12231,11 @@
         <v>467319</v>
       </c>
       <c r="G160">
-        <f>F160/1000</f>
+        <f t="shared" si="8"/>
         <v>467.31900000000002</v>
       </c>
       <c r="H160">
-        <f>G160/60</f>
+        <f t="shared" si="9"/>
         <v>7.7886500000000005</v>
       </c>
     </row>
@@ -12131,11 +12259,11 @@
         <v>255289</v>
       </c>
       <c r="G161">
-        <f>F161/1000</f>
+        <f t="shared" si="8"/>
         <v>255.28899999999999</v>
       </c>
       <c r="H161">
-        <f>G161/60</f>
+        <f t="shared" si="9"/>
         <v>4.2548166666666667</v>
       </c>
     </row>
@@ -12159,11 +12287,11 @@
         <v>173305</v>
       </c>
       <c r="G162">
-        <f>F162/1000</f>
+        <f t="shared" ref="G162:G193" si="10">F162/1000</f>
         <v>173.30500000000001</v>
       </c>
       <c r="H162">
-        <f>G162/60</f>
+        <f t="shared" ref="H162:H193" si="11">G162/60</f>
         <v>2.8884166666666666</v>
       </c>
     </row>
@@ -12187,11 +12315,11 @@
         <v>458850</v>
       </c>
       <c r="G163">
-        <f>F163/1000</f>
+        <f t="shared" si="10"/>
         <v>458.85</v>
       </c>
       <c r="H163">
-        <f>G163/60</f>
+        <f t="shared" si="11"/>
         <v>7.6475</v>
       </c>
     </row>
@@ -12215,11 +12343,11 @@
         <v>430740</v>
       </c>
       <c r="G164">
-        <f>F164/1000</f>
+        <f t="shared" si="10"/>
         <v>430.74</v>
       </c>
       <c r="H164">
-        <f>G164/60</f>
+        <f t="shared" si="11"/>
         <v>7.1790000000000003</v>
       </c>
     </row>
@@ -12243,11 +12371,11 @@
         <v>203585</v>
       </c>
       <c r="G165">
-        <f>F165/1000</f>
+        <f t="shared" si="10"/>
         <v>203.58500000000001</v>
       </c>
       <c r="H165">
-        <f>G165/60</f>
+        <f t="shared" si="11"/>
         <v>3.3930833333333337</v>
       </c>
     </row>
@@ -12271,11 +12399,11 @@
         <v>294459</v>
       </c>
       <c r="G166">
-        <f>F166/1000</f>
+        <f t="shared" si="10"/>
         <v>294.459</v>
       </c>
       <c r="H166">
-        <f>G166/60</f>
+        <f t="shared" si="11"/>
         <v>4.9076500000000003</v>
       </c>
     </row>
@@ -12299,11 +12427,11 @@
         <v>115398</v>
       </c>
       <c r="G167">
-        <f>F167/1000</f>
+        <f t="shared" si="10"/>
         <v>115.398</v>
       </c>
       <c r="H167">
-        <f>G167/60</f>
+        <f t="shared" si="11"/>
         <v>1.9233</v>
       </c>
     </row>
@@ -12327,11 +12455,11 @@
         <v>264490</v>
       </c>
       <c r="G168">
-        <f>F168/1000</f>
+        <f t="shared" si="10"/>
         <v>264.49</v>
       </c>
       <c r="H168">
-        <f>G168/60</f>
+        <f t="shared" si="11"/>
         <v>4.4081666666666672</v>
       </c>
     </row>
@@ -12355,11 +12483,11 @@
         <v>56055.199999999997</v>
       </c>
       <c r="G169">
-        <f>F169/1000</f>
+        <f t="shared" si="10"/>
         <v>56.055199999999999</v>
       </c>
       <c r="H169">
-        <f>G169/60</f>
+        <f t="shared" si="11"/>
         <v>0.93425333333333327</v>
       </c>
     </row>
@@ -12383,11 +12511,11 @@
         <v>289286</v>
       </c>
       <c r="G170">
-        <f>F170/1000</f>
+        <f t="shared" si="10"/>
         <v>289.286</v>
       </c>
       <c r="H170">
-        <f>G170/60</f>
+        <f t="shared" si="11"/>
         <v>4.8214333333333332</v>
       </c>
     </row>
@@ -12411,11 +12539,11 @@
         <v>74632.3</v>
       </c>
       <c r="G171">
-        <f>F171/1000</f>
+        <f t="shared" si="10"/>
         <v>74.632300000000001</v>
       </c>
       <c r="H171">
-        <f>G171/60</f>
+        <f t="shared" si="11"/>
         <v>1.2438716666666667</v>
       </c>
     </row>
@@ -12439,11 +12567,11 @@
         <v>115146</v>
       </c>
       <c r="G172">
-        <f>F172/1000</f>
+        <f t="shared" si="10"/>
         <v>115.146</v>
       </c>
       <c r="H172">
-        <f>G172/60</f>
+        <f t="shared" si="11"/>
         <v>1.9191</v>
       </c>
     </row>
@@ -12467,11 +12595,11 @@
         <v>364550</v>
       </c>
       <c r="G173">
-        <f>F173/1000</f>
+        <f t="shared" si="10"/>
         <v>364.55</v>
       </c>
       <c r="H173">
-        <f>G173/60</f>
+        <f t="shared" si="11"/>
         <v>6.0758333333333336</v>
       </c>
     </row>
@@ -12495,11 +12623,11 @@
         <v>1741.68</v>
       </c>
       <c r="G174">
-        <f>F174/1000</f>
+        <f t="shared" si="10"/>
         <v>1.7416800000000001</v>
       </c>
       <c r="H174">
-        <f>G174/60</f>
+        <f t="shared" si="11"/>
         <v>2.9028000000000002E-2</v>
       </c>
     </row>
@@ -12523,11 +12651,11 @@
         <v>34334.699999999997</v>
       </c>
       <c r="G175">
-        <f>F175/1000</f>
+        <f t="shared" si="10"/>
         <v>34.334699999999998</v>
       </c>
       <c r="H175">
-        <f>G175/60</f>
+        <f t="shared" si="11"/>
         <v>0.572245</v>
       </c>
     </row>
@@ -12551,11 +12679,11 @@
         <v>311581</v>
       </c>
       <c r="G176">
-        <f>F176/1000</f>
+        <f t="shared" si="10"/>
         <v>311.58100000000002</v>
       </c>
       <c r="H176">
-        <f>G176/60</f>
+        <f t="shared" si="11"/>
         <v>5.1930166666666668</v>
       </c>
     </row>
@@ -12579,11 +12707,11 @@
         <v>312315</v>
       </c>
       <c r="G177">
-        <f>F177/1000</f>
+        <f t="shared" si="10"/>
         <v>312.315</v>
       </c>
       <c r="H177">
-        <f>G177/60</f>
+        <f t="shared" si="11"/>
         <v>5.2052500000000004</v>
       </c>
     </row>
@@ -12607,11 +12735,11 @@
         <v>215878</v>
       </c>
       <c r="G178">
-        <f>F178/1000</f>
+        <f t="shared" si="10"/>
         <v>215.87799999999999</v>
       </c>
       <c r="H178">
-        <f>G178/60</f>
+        <f t="shared" si="11"/>
         <v>3.5979666666666663</v>
       </c>
     </row>
@@ -12635,11 +12763,11 @@
         <v>502064</v>
       </c>
       <c r="G179">
-        <f>F179/1000</f>
+        <f t="shared" si="10"/>
         <v>502.06400000000002</v>
       </c>
       <c r="H179">
-        <f>G179/60</f>
+        <f t="shared" si="11"/>
         <v>8.3677333333333337</v>
       </c>
     </row>
@@ -12663,11 +12791,11 @@
         <v>332330</v>
       </c>
       <c r="G180">
-        <f>F180/1000</f>
+        <f t="shared" si="10"/>
         <v>332.33</v>
       </c>
       <c r="H180">
-        <f>G180/60</f>
+        <f t="shared" si="11"/>
         <v>5.5388333333333328</v>
       </c>
     </row>
@@ -12691,11 +12819,11 @@
         <v>223424</v>
       </c>
       <c r="G181">
-        <f>F181/1000</f>
+        <f t="shared" si="10"/>
         <v>223.42400000000001</v>
       </c>
       <c r="H181">
-        <f>G181/60</f>
+        <f t="shared" si="11"/>
         <v>3.7237333333333336</v>
       </c>
     </row>
@@ -12719,11 +12847,11 @@
         <v>358829</v>
       </c>
       <c r="G182">
-        <f>F182/1000</f>
+        <f t="shared" si="10"/>
         <v>358.82900000000001</v>
       </c>
       <c r="H182">
-        <f>G182/60</f>
+        <f t="shared" si="11"/>
         <v>5.9804833333333338</v>
       </c>
     </row>
@@ -12747,11 +12875,11 @@
         <v>143159</v>
       </c>
       <c r="G183">
-        <f>F183/1000</f>
+        <f t="shared" si="10"/>
         <v>143.15899999999999</v>
       </c>
       <c r="H183">
-        <f>G183/60</f>
+        <f t="shared" si="11"/>
         <v>2.3859833333333333</v>
       </c>
     </row>
@@ -12775,11 +12903,11 @@
         <v>395.22300000000001</v>
       </c>
       <c r="G184">
-        <f>F184/1000</f>
+        <f t="shared" si="10"/>
         <v>0.39522299999999999</v>
       </c>
       <c r="H184">
-        <f>G184/60</f>
+        <f t="shared" si="11"/>
         <v>6.5870499999999997E-3</v>
       </c>
     </row>
@@ -12803,11 +12931,11 @@
         <v>102988</v>
       </c>
       <c r="G185">
-        <f>F185/1000</f>
+        <f t="shared" si="10"/>
         <v>102.988</v>
       </c>
       <c r="H185">
-        <f>G185/60</f>
+        <f t="shared" si="11"/>
         <v>1.7164666666666666</v>
       </c>
     </row>
@@ -12831,11 +12959,11 @@
         <v>43128.6</v>
       </c>
       <c r="G186">
-        <f>F186/1000</f>
+        <f t="shared" si="10"/>
         <v>43.128599999999999</v>
       </c>
       <c r="H186">
-        <f>G186/60</f>
+        <f t="shared" si="11"/>
         <v>0.71880999999999995</v>
       </c>
     </row>
@@ -12859,11 +12987,11 @@
         <v>254297</v>
       </c>
       <c r="G187">
-        <f>F187/1000</f>
+        <f t="shared" si="10"/>
         <v>254.297</v>
       </c>
       <c r="H187">
-        <f>G187/60</f>
+        <f t="shared" si="11"/>
         <v>4.2382833333333334</v>
       </c>
     </row>
@@ -12887,11 +13015,11 @@
         <v>1393.89</v>
       </c>
       <c r="G188">
-        <f>F188/1000</f>
+        <f t="shared" si="10"/>
         <v>1.3938900000000001</v>
       </c>
       <c r="H188">
-        <f>G188/60</f>
+        <f t="shared" si="11"/>
         <v>2.3231500000000002E-2</v>
       </c>
     </row>
@@ -12915,11 +13043,11 @@
         <v>373311</v>
       </c>
       <c r="G189">
-        <f>F189/1000</f>
+        <f t="shared" si="10"/>
         <v>373.31099999999998</v>
       </c>
       <c r="H189">
-        <f>G189/60</f>
+        <f t="shared" si="11"/>
         <v>6.2218499999999999</v>
       </c>
     </row>
@@ -12943,11 +13071,11 @@
         <v>433514</v>
       </c>
       <c r="G190">
-        <f>F190/1000</f>
+        <f t="shared" si="10"/>
         <v>433.51400000000001</v>
       </c>
       <c r="H190">
-        <f>G190/60</f>
+        <f t="shared" si="11"/>
         <v>7.2252333333333336</v>
       </c>
     </row>
@@ -12971,11 +13099,11 @@
         <v>298171</v>
       </c>
       <c r="G191">
-        <f>F191/1000</f>
+        <f t="shared" si="10"/>
         <v>298.17099999999999</v>
       </c>
       <c r="H191">
-        <f>G191/60</f>
+        <f t="shared" si="11"/>
         <v>4.9695166666666664</v>
       </c>
     </row>
@@ -12999,11 +13127,11 @@
         <v>72642.3</v>
       </c>
       <c r="G192">
-        <f>F192/1000</f>
+        <f t="shared" si="10"/>
         <v>72.642300000000006</v>
       </c>
       <c r="H192">
-        <f>G192/60</f>
+        <f t="shared" si="11"/>
         <v>1.2107050000000001</v>
       </c>
     </row>
@@ -13027,11 +13155,11 @@
         <v>149298</v>
       </c>
       <c r="G193">
-        <f>F193/1000</f>
+        <f t="shared" si="10"/>
         <v>149.298</v>
       </c>
       <c r="H193">
-        <f>G193/60</f>
+        <f t="shared" si="11"/>
         <v>2.4883000000000002</v>
       </c>
     </row>
@@ -13055,11 +13183,11 @@
         <v>274529</v>
       </c>
       <c r="G194">
-        <f>F194/1000</f>
+        <f t="shared" ref="G194:G225" si="12">F194/1000</f>
         <v>274.529</v>
       </c>
       <c r="H194">
-        <f>G194/60</f>
+        <f t="shared" ref="H194:H225" si="13">G194/60</f>
         <v>4.5754833333333336</v>
       </c>
     </row>
@@ -13083,11 +13211,11 @@
         <v>59938.2</v>
       </c>
       <c r="G195">
-        <f>F195/1000</f>
+        <f t="shared" si="12"/>
         <v>59.938199999999995</v>
       </c>
       <c r="H195">
-        <f>G195/60</f>
+        <f t="shared" si="13"/>
         <v>0.99896999999999991</v>
       </c>
     </row>
@@ -13111,11 +13239,11 @@
         <v>38235.599999999999</v>
       </c>
       <c r="G196">
-        <f>F196/1000</f>
+        <f t="shared" si="12"/>
         <v>38.235599999999998</v>
       </c>
       <c r="H196">
-        <f>G196/60</f>
+        <f t="shared" si="13"/>
         <v>0.63725999999999994</v>
       </c>
     </row>
@@ -13139,11 +13267,11 @@
         <v>257216</v>
       </c>
       <c r="G197">
-        <f>F197/1000</f>
+        <f t="shared" si="12"/>
         <v>257.21600000000001</v>
       </c>
       <c r="H197">
-        <f>G197/60</f>
+        <f t="shared" si="13"/>
         <v>4.2869333333333337</v>
       </c>
     </row>
@@ -13167,11 +13295,11 @@
         <v>422590</v>
       </c>
       <c r="G198">
-        <f>F198/1000</f>
+        <f t="shared" si="12"/>
         <v>422.59</v>
       </c>
       <c r="H198">
-        <f>G198/60</f>
+        <f t="shared" si="13"/>
         <v>7.0431666666666661</v>
       </c>
     </row>
@@ -13195,11 +13323,11 @@
         <v>450667</v>
       </c>
       <c r="G199">
-        <f>F199/1000</f>
+        <f t="shared" si="12"/>
         <v>450.66699999999997</v>
       </c>
       <c r="H199">
-        <f>G199/60</f>
+        <f t="shared" si="13"/>
         <v>7.5111166666666662</v>
       </c>
     </row>
@@ -13223,11 +13351,11 @@
         <v>234388</v>
       </c>
       <c r="G200">
-        <f>F200/1000</f>
+        <f t="shared" si="12"/>
         <v>234.38800000000001</v>
       </c>
       <c r="H200">
-        <f>G200/60</f>
+        <f t="shared" si="13"/>
         <v>3.9064666666666668</v>
       </c>
     </row>
@@ -13251,11 +13379,11 @@
         <v>125153</v>
       </c>
       <c r="G201">
-        <f>F201/1000</f>
+        <f t="shared" si="12"/>
         <v>125.15300000000001</v>
       </c>
       <c r="H201">
-        <f>G201/60</f>
+        <f t="shared" si="13"/>
         <v>2.0858833333333333</v>
       </c>
     </row>

</xml_diff>